<commit_message>
Fix to missing lesson 4
</commit_message>
<xml_diff>
--- a/Lesson_4-Temp_dis_progress_1/data/sample_data.xlsx
+++ b/Lesson_4-Temp_dis_progress_1/data/sample_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Professional\Side_projects\web_epidem\Lesson_4-Temp_dis_progress_1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D59CEDF9-DE2C-4AD9-B8FA-E9D0A850A8D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00CB328D-19B8-48D0-A1A1-383B7BD0013B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{D352B6AB-2D07-9149-B9C6-11BD235ECEA6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{D352B6AB-2D07-9149-B9C6-11BD235ECEA6}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
     <t>number_infected</t>
   </si>
   <si>
-    <t>day</t>
+    <t>day_after_infection</t>
   </si>
 </sst>
 </file>
@@ -415,8 +415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{641687BD-793B-8A46-876D-25387D356C13}">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -717,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38962C78-1C25-4D2E-9147-C7F70F54F859}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>